<commit_message>
select file 주석 처리
</commit_message>
<xml_diff>
--- a/설정.xlsx
+++ b/설정.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DmuDomitory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84C7495-F4A8-4431-A4BD-75D7AAF2CE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECF1B1E-042D-414D-8DDC-90E2E70CC091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{05F04895-7036-41FE-8EBE-498A70469EAD}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="19200" windowHeight="11170" xr2:uid="{05F04895-7036-41FE-8EBE-498A70469EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>